<commit_message>
re-run and update boro_4_analysis with new CZ shapes
</commit_message>
<xml_diff>
--- a/data-prep/cz summary statistics.xlsx
+++ b/data-prep/cz summary statistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrykanengiser/Documents/GitHub/fcny-community-solar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrykanengiser/Documents/GitHub/fcny-community-solar/data-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11BF88A-CD0C-B343-B527-8F5E8DDB8AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FF39ED-08DE-E943-AA2A-ADAD2ED07AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Low roof building</t>
   </si>
@@ -77,60 +77,21 @@
     <t>Neighborhood</t>
   </si>
   <si>
-    <t>Huge cluster, probably should be broken up into pieces to target outreach b/c of diversity of bldg type</t>
-  </si>
-  <si>
     <t>Number buildings</t>
   </si>
   <si>
-    <t>Lots of LL97 coverage, lots of solar energy, disadvantaged community</t>
-  </si>
-  <si>
-    <t>High suitability, poor solar generation</t>
-  </si>
-  <si>
-    <t>Little LL97 but good at everything else</t>
-  </si>
-  <si>
-    <t>Half LL97 coverage, highly suitable and good solar potential</t>
-  </si>
-  <si>
-    <t>Greenpoint (IBZ)</t>
-  </si>
-  <si>
     <t>North Brooklyn Waterfront</t>
   </si>
   <si>
-    <t>Flushing Ave/North Brooklyn IBZ</t>
-  </si>
-  <si>
-    <t>Fort Greene/BK Navy Yard</t>
-  </si>
-  <si>
-    <t>Red Hook</t>
-  </si>
-  <si>
-    <t>Crown Heights-Utica Ave</t>
-  </si>
-  <si>
     <t>East New York IBZ</t>
   </si>
   <si>
-    <t>East New York-Flatlands IBZ</t>
-  </si>
-  <si>
-    <t>Canarsie-Flatlands IBZ</t>
-  </si>
-  <si>
     <t>Sunset Park</t>
   </si>
   <si>
     <t>Prospect Park South</t>
   </si>
   <si>
-    <t>Sheepshead Bay-Nostrand Houses</t>
-  </si>
-  <si>
     <t>Henry ranking</t>
   </si>
   <si>
@@ -150,6 +111,30 @@
   </si>
   <si>
     <t>Percent sites meeting each flag (top three per row in green, top 3 per column bolded)</t>
+  </si>
+  <si>
+    <t>Greenpoint IBZ</t>
+  </si>
+  <si>
+    <t>Downtown BK/Naby Yard/North Brooklyn IBZ</t>
+  </si>
+  <si>
+    <t>Red Hook/Gowanus</t>
+  </si>
+  <si>
+    <t>East New York - Flatlands IBZ</t>
+  </si>
+  <si>
+    <t>Canarsie - Flatlands IBZ</t>
+  </si>
+  <si>
+    <t>Starrett City</t>
+  </si>
+  <si>
+    <t>Sheepshead Bay - Nostrand Houses</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -699,7 +684,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="20">
     <dxf>
       <font>
         <b/>
@@ -753,136 +738,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1324,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1338,9 +1193,9 @@
     <col min="5" max="16" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E1" s="6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -1351,9 +1206,9 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -1362,7 +1217,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -1395,663 +1250,668 @@
         <v>11</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D3">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4">
-        <v>0.76470588235294101</v>
+        <v>0.57142857142857095</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I3" s="4">
-        <v>0.52941176470588203</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="4">
-        <v>0.64705882352941102</v>
+        <v>0.78571428571428503</v>
       </c>
       <c r="K3" s="4">
-        <v>0.35294117647058798</v>
+        <v>0.42857142857142799</v>
       </c>
       <c r="L3" s="4">
-        <v>0.32352941176470501</v>
+        <v>0.35714285714285698</v>
       </c>
       <c r="M3" s="4">
         <v>1</v>
       </c>
       <c r="N3" s="2">
-        <v>7.23529411764705</v>
+        <v>7.21428571428571</v>
       </c>
       <c r="O3" s="2">
-        <v>395.09277325446999</v>
+        <v>458.25259319455699</v>
       </c>
       <c r="P3" s="2">
-        <v>6716.5771453259904</v>
+        <v>6415.5363047237997</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="E4" s="4">
-        <v>0.70253164556962</v>
+        <v>0.63333333333333297</v>
       </c>
       <c r="F4" s="4">
-        <v>0.810126582278481</v>
+        <v>0.85</v>
       </c>
       <c r="G4" s="4">
-        <v>8.8607594936708806E-2</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="H4" s="4">
-        <v>3.7974683544303799E-2</v>
+        <v>1.6666666666666601E-2</v>
       </c>
       <c r="I4" s="4">
-        <v>0.189873417721519</v>
-      </c>
-      <c r="J4" s="4"/>
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="K4" s="4">
-        <v>0.531645569620253</v>
+        <v>0.46666666666666601</v>
       </c>
       <c r="L4" s="4">
-        <v>0.316455696202531</v>
+        <v>0.35</v>
       </c>
       <c r="M4" s="4">
-        <v>0.822784810126582</v>
+        <v>0.91666666666666596</v>
       </c>
       <c r="N4" s="2">
-        <v>5.5569620253164498</v>
+        <v>5.5333333333333297</v>
       </c>
       <c r="O4" s="2">
-        <v>201.782456864989</v>
+        <v>217.69579286384501</v>
       </c>
       <c r="P4" s="3">
-        <v>15940.8140923342</v>
+        <v>13061.7475718307</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>622</v>
+        <v>896</v>
       </c>
       <c r="E5" s="4">
-        <v>0.71166134185303498</v>
+        <v>0.50446428571428503</v>
       </c>
       <c r="F5" s="4">
-        <v>0.71884984025559095</v>
+        <v>0.55022321428571397</v>
       </c>
       <c r="G5" s="4">
-        <v>0.18849840255590999</v>
-      </c>
-      <c r="H5" s="4"/>
+        <v>0.22767857142857101</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.1160714285714201E-3</v>
+      </c>
       <c r="I5" s="4">
-        <v>0.28354632587859402</v>
+        <v>0.32421875</v>
       </c>
       <c r="J5" s="4">
-        <v>0.76480000000000004</v>
+        <v>0.63169642857142805</v>
       </c>
       <c r="K5" s="4">
-        <v>0.52715654952076596</v>
+        <v>0.63727678571428503</v>
       </c>
       <c r="L5" s="4">
-        <v>0.25758785942492002</v>
+        <v>0.22572544642857101</v>
       </c>
       <c r="M5" s="4">
-        <v>0.99839999999999995</v>
+        <v>0.9140625</v>
       </c>
       <c r="N5" s="2">
-        <v>6.7428115015974397</v>
+        <v>6.15959821428571</v>
       </c>
       <c r="O5" s="2">
-        <v>232.553722842556</v>
+        <v>209.43789739707199</v>
       </c>
       <c r="P5" s="2">
-        <v>145578.63049944001</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>14</v>
+        <v>187656.35606777601</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D6">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="E6" s="4">
-        <v>0.26785714285714202</v>
+        <v>0.48514851485148502</v>
       </c>
       <c r="F6" s="4">
-        <v>0.30952380952380898</v>
+        <v>0.59405940594059403</v>
       </c>
       <c r="G6" s="4">
-        <v>0.30952380952380898</v>
-      </c>
-      <c r="H6" s="4"/>
+        <v>0.42574257425742501</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I6" s="4">
-        <v>0.57142857142857095</v>
+        <v>0.46039603960395997</v>
       </c>
       <c r="J6" s="4">
-        <v>0.238095238095238</v>
+        <v>0.26732673267326701</v>
       </c>
       <c r="K6" s="4">
-        <v>0.89285714285714202</v>
+        <v>0.58415841584158401</v>
       </c>
       <c r="L6" s="4">
-        <v>0.13095238095237999</v>
+        <v>0.235148514851485</v>
       </c>
       <c r="M6" s="4">
-        <v>0.84523809523809501</v>
+        <v>0.91089108910891003</v>
       </c>
       <c r="N6" s="2">
-        <v>5.6904761904761898</v>
+        <v>6.1980198019801902</v>
       </c>
       <c r="O6" s="2">
-        <v>148.70071473253699</v>
+        <v>242.670622097391</v>
       </c>
       <c r="P6" s="2">
-        <v>12490.860037533101</v>
+        <v>24509.7328318365</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="E7" s="4">
-        <v>0.54285714285714204</v>
+        <v>0.50632911392405</v>
       </c>
       <c r="F7" s="4">
-        <v>0.17142857142857101</v>
+        <v>0.670886075949367</v>
       </c>
       <c r="G7" s="4">
-        <v>0.82857142857142796</v>
-      </c>
-      <c r="H7" s="4"/>
+        <v>0.341772151898734</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I7" s="4">
-        <v>0.75714285714285701</v>
+        <v>0.341772151898734</v>
       </c>
       <c r="J7" s="4">
-        <v>0.65714285714285703</v>
+        <v>1</v>
       </c>
       <c r="K7" s="4">
-        <v>0.77142857142857102</v>
+        <v>0.556962025316455</v>
       </c>
       <c r="L7" s="4">
-        <v>0.2</v>
+        <v>0.31223628691983102</v>
       </c>
       <c r="M7" s="4">
         <v>1</v>
       </c>
       <c r="N7" s="3">
-        <v>7.2</v>
+        <v>6.7594936708860702</v>
       </c>
       <c r="O7" s="2">
-        <v>132.10079346843401</v>
+        <v>190.81368935165801</v>
       </c>
       <c r="P7" s="3">
-        <v>4623.5277713952</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>17</v>
+        <v>15074.281458781001</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D8">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E8" s="4">
-        <v>0.71153846153846101</v>
+        <v>0.89411764705882302</v>
       </c>
       <c r="F8" s="4">
-        <v>0.66666666666666596</v>
+        <v>0.89411764705882302</v>
       </c>
       <c r="G8" s="4">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="H8" s="4"/>
+        <v>9.41176470588235E-2</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I8" s="4">
-        <v>0.33974358974358898</v>
+        <v>0.252941176470588</v>
       </c>
       <c r="J8" s="4">
-        <v>1</v>
+        <v>0.65882352941176403</v>
       </c>
       <c r="K8" s="4">
-        <v>0.55128205128205099</v>
+        <v>0.36470588235294099</v>
       </c>
       <c r="L8" s="4">
-        <v>0.316239316239316</v>
+        <v>0.34411764705882297</v>
       </c>
       <c r="M8" s="4">
         <v>1</v>
       </c>
       <c r="N8" s="2">
-        <v>7.1538461538461497</v>
+        <v>7.0470588235294098</v>
       </c>
       <c r="O8" s="2">
-        <v>188.43895880632101</v>
+        <v>313.210042665044</v>
       </c>
       <c r="P8" s="3">
-        <v>14698.2387868931</v>
+        <v>26622.853626528798</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D9">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E9" s="4">
-        <v>0.63888888888888795</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.52777777777777701</v>
+      </c>
       <c r="G9" s="4">
-        <v>5.5555555555555497E-2</v>
-      </c>
-      <c r="H9" s="4"/>
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I9" s="4">
-        <v>5.5555555555555497E-2</v>
+        <v>0.52777777777777701</v>
       </c>
       <c r="J9" s="4">
-        <v>0.66666666666666596</v>
+        <v>1</v>
       </c>
       <c r="K9" s="4">
         <v>0.83333333333333304</v>
       </c>
       <c r="L9" s="4">
-        <v>0.41666666666666602</v>
+        <v>0.29166666666666602</v>
       </c>
       <c r="M9" s="4">
-        <v>0.66666666666666596</v>
+        <v>1</v>
       </c>
       <c r="N9" s="2">
-        <v>5.2777777777777697</v>
+        <v>7.7777777777777697</v>
       </c>
       <c r="O9" s="2">
-        <v>154.16015110869401</v>
+        <v>465.94659597514402</v>
       </c>
       <c r="P9" s="3">
-        <v>2774.8827199564998</v>
+        <v>16774.0774551051</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D10">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="E10" s="4">
-        <v>0.952380952380952</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.90476190476190399</v>
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="G10" s="4">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="H10" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I10" s="4">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
       <c r="J10" s="4">
-        <v>0.65476190476190399</v>
+        <v>1</v>
       </c>
       <c r="K10" s="4">
-        <v>0.35714285714285698</v>
+        <v>1</v>
       </c>
       <c r="L10" s="4">
-        <v>0.34523809523809501</v>
+        <v>0.2</v>
       </c>
       <c r="M10" s="4">
         <v>1</v>
       </c>
       <c r="N10" s="2">
-        <v>7.1428571428571397</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="O10" s="2">
-        <v>314.47683401946102</v>
+        <v>126.73994730464</v>
       </c>
       <c r="P10" s="3">
-        <v>26416.054057634799</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>18</v>
+        <v>1267.3994730464001</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="E11" s="4">
-        <v>0.66176470588235203</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.38235294117647001</v>
+        <v>0.107913669064748</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="G11" s="4">
-        <v>0.61764705882352899</v>
-      </c>
-      <c r="H11" s="4"/>
+        <v>3.5971223021582698E-2</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I11" s="4">
-        <v>0.64705882352941102</v>
+        <v>4.31654676258992E-2</v>
       </c>
       <c r="J11" s="4">
-        <v>1</v>
+        <v>0.74820143884891999</v>
       </c>
       <c r="K11" s="4">
-        <v>0.91176470588235203</v>
+        <v>0.85611510791366896</v>
       </c>
       <c r="L11" s="4">
-        <v>0.27941176470588203</v>
+        <v>0.27697841726618699</v>
       </c>
       <c r="M11" s="4">
-        <v>0.97058823529411697</v>
+        <v>0.43884892086330901</v>
       </c>
       <c r="N11" s="2">
-        <v>8.5294117647058805</v>
+        <v>3.7913669064748201</v>
       </c>
       <c r="O11" s="2">
-        <v>511.001848279711</v>
+        <v>121.17875409410399</v>
       </c>
       <c r="P11" s="3">
-        <v>17374.0628415102</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>16</v>
+        <v>16843.8468190805</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D12">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E12" s="4">
-        <v>0.72164948453608202</v>
+        <v>0.52083333333333304</v>
       </c>
       <c r="F12" s="4">
-        <v>0.96907216494845305</v>
+        <v>0.97916666666666596</v>
       </c>
       <c r="G12" s="4">
-        <v>3.0927835051546299E-2</v>
-      </c>
-      <c r="H12" s="4"/>
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I12" s="4">
-        <v>0.15463917525773099</v>
+        <v>0.15104166666666599</v>
       </c>
       <c r="J12" s="4">
-        <v>0.49484536082474201</v>
+        <v>0.48958333333333298</v>
       </c>
       <c r="K12" s="4">
-        <v>0.50515463917525705</v>
+        <v>0.51041666666666596</v>
       </c>
       <c r="L12" s="4">
-        <v>0.32731958762886598</v>
+        <v>0.33072916666666602</v>
       </c>
       <c r="M12" s="4">
         <v>1</v>
       </c>
       <c r="N12" s="3">
-        <v>6.5670103092783503</v>
+        <v>6.1770833333333304</v>
       </c>
       <c r="O12" s="2">
-        <v>307.833211980155</v>
+        <v>310.01414672821301</v>
       </c>
       <c r="P12" s="3">
-        <v>29859.8215620751</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>19</v>
+        <v>29761.358085908501</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13">
-        <v>218</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.55555555555555503</v>
-      </c>
-      <c r="F13" s="4">
-        <v>3.3816425120772903E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="G13" s="4">
-        <v>9.6618357487922704E-2</v>
-      </c>
-      <c r="H13" s="4">
-        <v>4.8309178743961298E-3</v>
+        <v>1</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="I13" s="4">
-        <v>6.0386473429951598E-2</v>
+        <v>0.95</v>
       </c>
       <c r="J13" s="4">
-        <v>0.69565217391304301</v>
+        <v>0.9</v>
       </c>
       <c r="K13" s="4">
-        <v>0.84057971014492705</v>
+        <v>1</v>
       </c>
       <c r="L13" s="4">
-        <v>0.14251207729468501</v>
+        <v>0.1</v>
       </c>
       <c r="M13" s="4">
-        <v>0.352657004830917</v>
+        <v>0.9</v>
       </c>
       <c r="N13" s="2">
-        <v>4.6666666666666599</v>
+        <v>6.9</v>
       </c>
       <c r="O13" s="2">
-        <v>127.408776517435</v>
+        <v>99.017945033580006</v>
       </c>
       <c r="P13" s="3">
-        <v>26373.6167391091</v>
+        <v>990.17945033579997</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>12</v>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D14">
-        <v>22</v>
+        <v>5744</v>
       </c>
       <c r="E14" s="5">
-        <v>0.52</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5">
-        <v>1</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5">
-        <v>0.98</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="K14" s="5">
-        <v>0.96</v>
-      </c>
-      <c r="L14" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="M14" s="5">
-        <v>0.72</v>
-      </c>
-      <c r="N14" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="O14" s="3">
-        <v>86.767851440656003</v>
-      </c>
-      <c r="P14" s="3">
-        <v>2169.1962860163999</v>
+        <v>0.35236768802228402</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.20961002785515301</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.51793175487465104</v>
+      </c>
+      <c r="H14" s="5">
+        <v>3.1685236768802201E-2</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.22684540389972099</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.54073816155988796</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0.685410863509749</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.19542130919219999</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0.45055710306406599</v>
+      </c>
+      <c r="N14" s="2">
+        <v>5.0614554317548697</v>
+      </c>
+      <c r="O14" s="2">
+        <v>185.027727026457</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1062799.26403997</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>5869</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0.58986096982027802</v>
+        <v>7270</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.38184319119669802</v>
       </c>
       <c r="F15" s="4">
-        <v>0.21447948457104099</v>
+        <v>0.28390646492434601</v>
       </c>
       <c r="G15" s="4">
-        <v>0.51135978297728002</v>
-      </c>
-      <c r="H15" s="5">
-        <v>3.0518819938962299E-2</v>
+        <v>0.45474552957358999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2.53094910591471E-2</v>
       </c>
       <c r="I15" s="4">
-        <v>0.23677517802644901</v>
+        <v>0.24291609353507501</v>
       </c>
       <c r="J15" s="4">
-        <v>0.52986087546657601</v>
+        <v>0.55722145804676704</v>
       </c>
       <c r="K15" s="4">
-        <v>0.68786029162427897</v>
+        <v>0.67317744154057702</v>
       </c>
       <c r="L15" s="4">
-        <v>0.1965496778569</v>
+        <v>0.203576341127922</v>
       </c>
       <c r="M15" s="4">
-        <v>0.464370546318289</v>
-      </c>
-      <c r="N15" s="2">
-        <v>5.5651068158697798</v>
-      </c>
-      <c r="O15" s="2">
-        <v>186.30325180628299</v>
-      </c>
-      <c r="P15" s="2">
-        <v>1098816.57915346</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>7282</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0.60450425707223199</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.28426256522933202</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0.45303488052732699</v>
-      </c>
-      <c r="H16" s="4">
-        <v>2.5267783575940599E-2</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0.24649821477615999</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0.55599835096880501</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0.67330403735237498</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0.20354984894259801</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0.541981585818331</v>
-      </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
+        <v>0.54250343878954599</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P14">
-    <sortCondition ref="B3:B14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P13">
+    <sortCondition ref="B3:B13"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="E1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:D14">
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="E3:M3">
+    <cfRule type="top10" dxfId="19" priority="27" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:M4">
+    <cfRule type="top10" dxfId="18" priority="26" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:M5">
+    <cfRule type="top10" dxfId="17" priority="25" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:M6">
+    <cfRule type="top10" dxfId="16" priority="24" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:M7">
+    <cfRule type="top10" dxfId="15" priority="23" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:M8">
+    <cfRule type="top10" dxfId="14" priority="22" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:M9">
+    <cfRule type="top10" dxfId="13" priority="21" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:M10">
+    <cfRule type="top10" dxfId="12" priority="20" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:M11">
+    <cfRule type="top10" dxfId="11" priority="19" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:M12">
+    <cfRule type="top10" dxfId="10" priority="18" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13:M13">
+    <cfRule type="top10" dxfId="9" priority="17" stopIfTrue="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D13">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2060,44 +1920,35 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:M3">
-    <cfRule type="top10" dxfId="20" priority="27" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:M4">
-    <cfRule type="top10" dxfId="19" priority="26" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:M5">
-    <cfRule type="top10" dxfId="18" priority="25" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6:M6">
-    <cfRule type="top10" dxfId="17" priority="24" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:M7">
-    <cfRule type="top10" dxfId="16" priority="23" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8:M8">
-    <cfRule type="top10" dxfId="15" priority="22" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:M9">
-    <cfRule type="top10" dxfId="14" priority="21" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10:M10">
-    <cfRule type="top10" dxfId="13" priority="20" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11:M11">
-    <cfRule type="top10" dxfId="12" priority="19" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:M12">
-    <cfRule type="top10" dxfId="11" priority="18" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13:M13">
-    <cfRule type="top10" dxfId="10" priority="17" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:M14">
-    <cfRule type="top10" dxfId="9" priority="16" stopIfTrue="1" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N14">
-    <cfRule type="colorScale" priority="29">
+  <conditionalFormatting sqref="E3:E13">
+    <cfRule type="top10" dxfId="8" priority="33" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F13">
+    <cfRule type="top10" dxfId="7" priority="34" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G13">
+    <cfRule type="top10" dxfId="6" priority="35" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H13">
+    <cfRule type="top10" dxfId="5" priority="36" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I13">
+    <cfRule type="top10" dxfId="4" priority="37" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J13">
+    <cfRule type="top10" dxfId="3" priority="38" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K13">
+    <cfRule type="top10" dxfId="2" priority="39" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L13">
+    <cfRule type="top10" dxfId="1" priority="40" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M13">
+    <cfRule type="top10" dxfId="0" priority="41" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N13">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2106,8 +1957,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O14">
-    <cfRule type="colorScale" priority="31">
+  <conditionalFormatting sqref="O3:O13">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2116,8 +1967,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P14">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="P3:P13">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2126,33 +1977,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E14">
-    <cfRule type="top10" dxfId="8" priority="9" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F14">
-    <cfRule type="top10" dxfId="7" priority="8" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G14">
-    <cfRule type="top10" dxfId="6" priority="7" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H14">
-    <cfRule type="top10" dxfId="5" priority="6" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I14">
-    <cfRule type="top10" dxfId="4" priority="5" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J14">
-    <cfRule type="top10" dxfId="3" priority="4" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K14">
-    <cfRule type="top10" dxfId="2" priority="3" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L14">
-    <cfRule type="top10" dxfId="1" priority="2" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M14">
-    <cfRule type="top10" dxfId="0" priority="1" rank="3"/>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>